<commit_message>
Updated documents from 'master' branch, added methods to session
</commit_message>
<xml_diff>
--- a/Project Pink/doc/scrum/scrum.xlsx
+++ b/Project Pink/doc/scrum/scrum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="466" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="341" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -144,15 +144,24 @@
     <t>Session save &amp; load</t>
   </si>
   <si>
+    <t>Load and save a Session</t>
+  </si>
+  <si>
     <t>Session memento</t>
   </si>
   <si>
+    <t>implement memento Pattern</t>
+  </si>
+  <si>
     <t>Fränzi</t>
   </si>
   <si>
     <t>Patient selection</t>
   </si>
   <si>
+    <t>Show patient information</t>
+  </si>
+  <si>
     <t>UI</t>
   </si>
   <si>
@@ -162,10 +171,13 @@
     <t>Patient session information</t>
   </si>
   <si>
+    <t>Show patient session information</t>
+  </si>
+  <si>
     <t>Memento pattern design</t>
   </si>
   <si>
-    <t>Prepare Presentation for Memento pattern </t>
+    <t>Prepare Presentation for Memento pattern</t>
   </si>
   <si>
     <t>-</t>
@@ -261,7 +273,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
@@ -276,7 +288,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -361,15 +372,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.86666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.2156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.4235294117647"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.3921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7607843137255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2549019607843"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.90588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.87843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.5607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.42352941176471"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2980392156863"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.678431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.94117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="28" outlineLevel="0" r="1" s="2">
@@ -541,22 +552,22 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10"/>
+      <selection activeCell="D9" activeCellId="0" pane="topLeft" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.21176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.05490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5686274509804"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.6196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9490196078431"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4352941176471"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.5921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.89019607843137"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7098039215686"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.0509803921569"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.9725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.90588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.23921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.08627450980392"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.2745098039216"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0039215686275"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6352941176471"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.92156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7607843137255"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.1098039215686"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.0470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.94117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="1" s="5">
@@ -662,7 +673,6 @@
       <c r="G4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
@@ -675,7 +685,7 @@
         <v>41</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>33</v>
@@ -695,19 +705,22 @@
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
         <v>1.6</v>
       </c>
@@ -715,19 +728,22 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
         <v>1.7</v>
       </c>
@@ -735,19 +751,22 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
         <v>1.8</v>
       </c>
@@ -755,22 +774,22 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>1.9</v>
       </c>

</xml_diff>

<commit_message>
Updated scrum documen - Reassigned task to Fränzi, since she wanted to do some programming
</commit_message>
<xml_diff>
--- a/Project Pink/doc/scrum/scrum.xlsx
+++ b/Project Pink/doc/scrum/scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1560" windowWidth="25600" windowHeight="17480" tabRatio="341" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="341" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -761,7 +761,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="35" style="1" customWidth="1"/>
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1425,7 +1425,7 @@
         <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
         <v>18</v>
@@ -1483,7 +1483,7 @@
         <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updated scrum document and did some cleaning up
</commit_message>
<xml_diff>
--- a/Project Pink/doc/scrum/scrum.xlsx
+++ b/Project Pink/doc/scrum/scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="341" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="341" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -263,6 +263,18 @@
   </si>
   <si>
     <t>Compile a list of medication, ingredients, allergies as preparation for task 2.2</t>
+  </si>
+  <si>
+    <t>10h</t>
+  </si>
+  <si>
+    <t>Figure out navigation for Vaadin Framework</t>
+  </si>
+  <si>
+    <t>Basic GUI, navigation between pages</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -758,7 +770,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -842,7 +854,7 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="70" customHeight="1">
@@ -918,10 +930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1306,10 +1318,10 @@
         <v>60</v>
       </c>
       <c r="I12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" t="s">
         <v>61</v>
-      </c>
-      <c r="J12" t="s">
-        <v>11</v>
       </c>
       <c r="K12" t="s">
         <v>57</v>
@@ -1378,6 +1390,12 @@
       <c r="I14" t="s">
         <v>58</v>
       </c>
+      <c r="J14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="28">
       <c r="A15">
@@ -1405,7 +1423,13 @@
         <v>74</v>
       </c>
       <c r="I15" t="s">
-        <v>74</v>
+        <v>58</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="28">
@@ -1436,10 +1460,16 @@
       <c r="I16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="28">
+      <c r="J16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="28">
       <c r="A17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1465,8 +1495,14 @@
       <c r="I17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="42">
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="42">
       <c r="A18">
         <v>2.5</v>
       </c>
@@ -1493,6 +1529,47 @@
       </c>
       <c r="I18" t="s">
         <v>68</v>
+      </c>
+      <c r="J18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="28">
+      <c r="A19">
+        <v>0.2</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
+        <v>59</v>
+      </c>
+      <c r="K19" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Scrum, diary and topics of the presentation
</commit_message>
<xml_diff>
--- a/Project Pink/doc/scrum/scrum.xlsx
+++ b/Project Pink/doc/scrum/scrum.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="0" windowWidth="25040" windowHeight="17560" tabRatio="341" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="341" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint Backlog'!$A$1:$K$31</definedName>
+  </definedNames>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -79,9 +82,6 @@
     <t>medium</t>
   </si>
   <si>
-    <t>3h</t>
-  </si>
-  <si>
     <t>Generate reports</t>
   </si>
   <si>
@@ -91,9 +91,6 @@
     <t>low</t>
   </si>
   <si>
-    <t>4h</t>
-  </si>
-  <si>
     <t>Integration of external systems</t>
   </si>
   <si>
@@ -196,39 +193,18 @@
     <t>Work In Progress</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>5h</t>
-  </si>
-  <si>
     <t>8h</t>
   </si>
   <si>
-    <t>22h</t>
-  </si>
-  <si>
     <t>20h</t>
   </si>
   <si>
-    <t>30h</t>
-  </si>
-  <si>
-    <t>35h</t>
-  </si>
-  <si>
     <t>Allergy Database</t>
   </si>
   <si>
     <t>Create DB table and entities for Allergies</t>
   </si>
   <si>
-    <t>0.5h</t>
-  </si>
-  <si>
     <t>Create test data for database (all databases) with patients, allergies, medicine, ingredients, a few sessions and doctors</t>
   </si>
   <si>
@@ -244,9 +220,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>7.5h</t>
-  </si>
-  <si>
     <t>Medication prescription</t>
   </si>
   <si>
@@ -265,18 +238,12 @@
     <t>Compile a list of medication, ingredients, allergies as preparation for task 2.2</t>
   </si>
   <si>
-    <t>10h</t>
-  </si>
-  <si>
     <t>Figure out navigation for Vaadin Framework</t>
   </si>
   <si>
     <t>Basic GUI, navigation between pages</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Search function</t>
   </si>
   <si>
@@ -314,6 +281,96 @@
   </si>
   <si>
     <t>Waiting</t>
+  </si>
+  <si>
+    <t>Continued in Sprint 3</t>
+  </si>
+  <si>
+    <t>Unit Tests MedicalService</t>
+  </si>
+  <si>
+    <t>Unit Tests SessionState</t>
+  </si>
+  <si>
+    <t>Create note for session</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>GUI Streamlining</t>
+  </si>
+  <si>
+    <t>Report all patients</t>
+  </si>
+  <si>
+    <t>Report medication</t>
+  </si>
+  <si>
+    <t>Mock datasource and Unit Tests for medical prescription</t>
+  </si>
+  <si>
+    <t>Unit tests for correct session state transitions and permissions</t>
+  </si>
+  <si>
+    <t>Allow the user to add a note to a session</t>
+  </si>
+  <si>
+    <t>General GUI streamlining, best effort</t>
+  </si>
+  <si>
+    <t>Allow the doctor to generate a report with all patients and the number of treatments / prescription per patient</t>
+  </si>
+  <si>
+    <t>Allow the doctor to generate a report with all available medication, ingredients and known sideeffects</t>
+  </si>
+  <si>
+    <t>Effort Plan Original [h]</t>
+  </si>
+  <si>
+    <t>Effort Plan Updated [h]</t>
+  </si>
+  <si>
+    <t>Effort Actual [h]</t>
+  </si>
+  <si>
+    <t>33h</t>
+  </si>
+  <si>
+    <t>42h</t>
+  </si>
+  <si>
+    <t>26.5h</t>
+  </si>
+  <si>
+    <t>25h</t>
+  </si>
+  <si>
+    <t>16h</t>
+  </si>
+  <si>
+    <t>37h</t>
+  </si>
+  <si>
+    <t>7h</t>
+  </si>
+  <si>
+    <t>Generic Software Engineering</t>
+  </si>
+  <si>
+    <t>critical</t>
+  </si>
+  <si>
+    <t>18h</t>
+  </si>
+  <si>
+    <t>5.5h</t>
+  </si>
+  <si>
+    <t>General software engineering tasks such as environment setup, navigation, Unit tests</t>
   </si>
 </sst>
 </file>
@@ -376,8 +433,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -404,15 +465,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -810,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -862,16 +927,16 @@
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="70" customHeight="1">
@@ -888,16 +953,16 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="70" customHeight="1">
@@ -913,11 +978,17 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="42" customHeight="1">
@@ -925,13 +996,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
@@ -945,19 +1016,45 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -973,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -990,31 +1087,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>7</v>
@@ -1028,31 +1125,31 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" t="s">
         <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" t="s">
-        <v>58</v>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28">
@@ -1063,31 +1160,31 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" t="s">
-        <v>58</v>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1098,31 +1195,31 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" t="s">
-        <v>58</v>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1133,31 +1230,31 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" t="s">
-        <v>59</v>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1168,31 +1265,31 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
         <v>42</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1203,31 +1300,31 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" t="s">
         <v>46</v>
       </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
       <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="28">
@@ -1238,31 +1335,31 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
       </c>
       <c r="K8" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="28">
@@ -1273,509 +1370,775 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
       </c>
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" t="s">
-        <v>58</v>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="13.25" customHeight="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="13.25" customHeight="1">
+      <c r="A10">
+        <v>1.6</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28">
       <c r="A11">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" t="s">
         <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
       </c>
-      <c r="H11" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" t="s">
-        <v>23</v>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="28">
       <c r="A12">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+      <c r="J12">
+        <v>0.5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="70">
+      <c r="A13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I12" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="28">
-      <c r="A13">
-        <v>2.1</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="28">
+      <c r="A14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
         <v>10</v>
       </c>
-      <c r="H13" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="70">
-      <c r="A14">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" t="s">
-        <v>58</v>
+      <c r="H14">
+        <v>7.5</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
       </c>
       <c r="K14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="28">
       <c r="A15">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="28">
       <c r="A16">
-        <v>2.4</v>
+        <v>0.1</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" t="s">
-        <v>47</v>
+        <v>68</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
       </c>
       <c r="K16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="28">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="42">
       <c r="A17">
-        <v>0.1</v>
+        <v>2.5</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="I17">
+        <v>0.5</v>
+      </c>
+      <c r="J17">
+        <v>0.5</v>
+      </c>
+      <c r="K17" t="s">
         <v>53</v>
       </c>
-      <c r="F17" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="42">
+    </row>
+    <row r="18" spans="1:11" ht="28">
       <c r="A18">
-        <v>2.5</v>
+        <v>0.2</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="42">
+      <c r="A19">
+        <v>2.6</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
         <v>53</v>
-      </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" t="s">
-        <v>68</v>
-      </c>
-      <c r="J18" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="28">
-      <c r="A19">
-        <v>0.2</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" t="s">
-        <v>59</v>
-      </c>
-      <c r="K19" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="42">
       <c r="A20">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="42">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="28">
       <c r="A21">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G21" t="s">
         <v>18</v>
       </c>
-      <c r="H21" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" t="s">
-        <v>58</v>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="28">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="42">
       <c r="A22">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
       </c>
       <c r="K22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="42">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="28">
       <c r="A23">
-        <v>3.2</v>
+        <v>0.3</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E23" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23" t="s">
-        <v>58</v>
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>2.5</v>
       </c>
       <c r="K23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="28">
       <c r="A24">
-        <v>0.3</v>
+        <v>2.4</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24">
+        <v>6</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="K24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="28">
+      <c r="A25">
+        <v>3.1</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="28">
+      <c r="A26">
+        <v>0.4</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="42">
+      <c r="A27">
+        <v>0.4</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="28">
+      <c r="A28">
+        <v>3.3</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="D28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="28">
+      <c r="A29">
+        <v>0.5</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" t="s">
         <v>10</v>
       </c>
-      <c r="H24" t="s">
-        <v>58</v>
-      </c>
-      <c r="I24" t="s">
-        <v>58</v>
-      </c>
-      <c r="K24" t="s">
-        <v>97</v>
+      <c r="H29">
+        <v>6</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="56">
+      <c r="A30">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" t="s">
+        <v>91</v>
+      </c>
+      <c r="K30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="56">
+      <c r="A31">
+        <v>4.2</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K31" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K31"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Updated scrum document (fixed numbering), added topics for presentation
</commit_message>
<xml_diff>
--- a/Project Pink/doc/scrum/scrum.xlsx
+++ b/Project Pink/doc/scrum/scrum.xlsx
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1919,7 +1919,7 @@
         <v>2</v>
       </c>
       <c r="K24" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="28">
@@ -1954,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="28">
@@ -1994,7 +1994,7 @@
     </row>
     <row r="27" spans="1:11" ht="42">
       <c r="A27">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="B27">
         <v>3</v>

</xml_diff>

<commit_message>
Updated Scrum document with latest inputs
</commit_message>
<xml_diff>
--- a/Project Pink/doc/scrum/scrum.xlsx
+++ b/Project Pink/doc/scrum/scrum.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint Backlog'!$A$1:$K$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint Backlog'!$A$1:$K$36</definedName>
   </definedNames>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="127">
   <si>
     <t>ID</t>
   </si>
@@ -398,6 +398,12 @@
   </si>
   <si>
     <t>0.10</t>
+  </si>
+  <si>
+    <t>Show warnings in SessionView</t>
+  </si>
+  <si>
+    <t>Show Warnings in SessionView</t>
   </si>
 </sst>
 </file>
@@ -1112,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2098,10 +2104,10 @@
         <v>1</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="28">
@@ -2133,7 +2139,7 @@
         <v>6</v>
       </c>
       <c r="J29">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="K29" t="s">
         <v>55</v>
@@ -2279,43 +2285,78 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="56">
-      <c r="A34">
-        <v>4.0999999999999996</v>
+    <row r="34" spans="1:11" ht="28">
+      <c r="A34" s="7">
+        <v>3.4</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E34" t="s">
-        <v>91</v>
+        <v>126</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
       </c>
       <c r="K34" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="56">
       <c r="A35">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
         <v>91</v>
       </c>
       <c r="K35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="56">
+      <c r="A36">
+        <v>4.2</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" t="s">
+        <v>91</v>
+      </c>
+      <c r="K36" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated scrum document with burndown chart
</commit_message>
<xml_diff>
--- a/Project Pink/doc/scrum/scrum.xlsx
+++ b/Project Pink/doc/scrum/scrum.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="341" activeTab="1"/>
+    <workbookView xWindow="1660" yWindow="880" windowWidth="25600" windowHeight="16060" tabRatio="341" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Burndown Chart" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint Backlog'!$A$1:$K$36</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -404,6 +405,18 @@
   </si>
   <si>
     <t>Show Warnings in SessionView</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Ideal</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Actual</t>
   </si>
 </sst>
 </file>
@@ -457,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -465,8 +478,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -486,8 +508,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -506,8 +538,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -517,6 +556,11 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -526,6 +570,11 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -599,6 +648,361 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown Chart - Project Pink</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$B$39:$C$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal 101.50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$D$38:$P$38</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>41398.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41402.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41410.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41411.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41416.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41418.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41423.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41425.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41427.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41430.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41432.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41437.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41439.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$D$39:$P$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>93.69230769230769</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85.88461538461538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.07692307692308</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.26923076923077</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.46153846153846</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.65384615384615</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46.84615384615384</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.03846153846154</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.42307692307692</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.61538461538461</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.807692307692306</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$B$40:$C$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual 101.50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$D$38:$P$38</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>41398.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41402.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41410.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41411.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41416.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41418.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41423.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41425.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41427.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41430.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41432.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41437.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41439.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$D$40:$P$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="4">
+                  <c:v>69.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2083303944"/>
+        <c:axId val="-2064237912"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2083303944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2064237912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2064237912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2083303944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1120,8 +1524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2370,4 +2774,1393 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="9">
+        <v>41398</v>
+      </c>
+      <c r="E1" s="9">
+        <v>41402</v>
+      </c>
+      <c r="F1" s="9">
+        <v>41410</v>
+      </c>
+      <c r="G1" s="9">
+        <v>41411</v>
+      </c>
+      <c r="H1" s="9">
+        <v>41416</v>
+      </c>
+      <c r="I1" s="9">
+        <v>41418</v>
+      </c>
+      <c r="J1" s="9">
+        <v>41423</v>
+      </c>
+      <c r="K1" s="9">
+        <v>41425</v>
+      </c>
+      <c r="L1" s="9">
+        <v>41427</v>
+      </c>
+      <c r="M1" s="9">
+        <v>41430</v>
+      </c>
+      <c r="N1" s="9">
+        <v>41432</v>
+      </c>
+      <c r="O1" s="9">
+        <v>41437</v>
+      </c>
+      <c r="P1" s="9">
+        <v>41439</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <f>'Sprint Backlog'!B2</f>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>'Sprint Backlog'!A2</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2">
+        <f>'Sprint Backlog'!H2</f>
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <f>'Sprint Backlog'!B3</f>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>'Sprint Backlog'!A3</f>
+        <v>1.2</v>
+      </c>
+      <c r="C3">
+        <f>'Sprint Backlog'!H3</f>
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
+        <f>'Sprint Backlog'!B4</f>
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>'Sprint Backlog'!A4</f>
+        <v>1.3</v>
+      </c>
+      <c r="C4">
+        <f>'Sprint Backlog'!H4</f>
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <f>'Sprint Backlog'!B5</f>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f>'Sprint Backlog'!A5</f>
+        <v>1.4</v>
+      </c>
+      <c r="C5">
+        <f>'Sprint Backlog'!H5</f>
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <f>'Sprint Backlog'!B6</f>
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f>'Sprint Backlog'!A6</f>
+        <v>1.5</v>
+      </c>
+      <c r="C6">
+        <f>'Sprint Backlog'!H6</f>
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <f>'Sprint Backlog'!B7</f>
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <f>'Sprint Backlog'!A7</f>
+        <v>1.6</v>
+      </c>
+      <c r="C7">
+        <f>'Sprint Backlog'!H7</f>
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8">
+        <f>'Sprint Backlog'!B8</f>
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>'Sprint Backlog'!A8</f>
+        <v>1.7</v>
+      </c>
+      <c r="C8">
+        <f>'Sprint Backlog'!H8</f>
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9">
+        <f>'Sprint Backlog'!B9</f>
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <f>'Sprint Backlog'!A9</f>
+        <v>1.8</v>
+      </c>
+      <c r="C9">
+        <f>'Sprint Backlog'!H9</f>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10">
+        <f>'Sprint Backlog'!B10</f>
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <f>'Sprint Backlog'!A10</f>
+        <v>1.6</v>
+      </c>
+      <c r="C10">
+        <f>'Sprint Backlog'!H10</f>
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11">
+        <f>'Sprint Backlog'!B11</f>
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <f>'Sprint Backlog'!A11</f>
+        <v>1.7</v>
+      </c>
+      <c r="C11">
+        <f>'Sprint Backlog'!H11</f>
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12">
+        <f>'Sprint Backlog'!B12</f>
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <f>'Sprint Backlog'!A12</f>
+        <v>2.1</v>
+      </c>
+      <c r="C12">
+        <f>'Sprint Backlog'!H12</f>
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0.5</v>
+      </c>
+      <c r="L12">
+        <v>0.5</v>
+      </c>
+      <c r="M12">
+        <v>0.5</v>
+      </c>
+      <c r="N12">
+        <v>0.5</v>
+      </c>
+      <c r="O12">
+        <v>0.5</v>
+      </c>
+      <c r="P12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <f>'Sprint Backlog'!B13</f>
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f>'Sprint Backlog'!A13</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C13">
+        <f>'Sprint Backlog'!H13</f>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14">
+        <f>'Sprint Backlog'!B14</f>
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <f>'Sprint Backlog'!A14</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C14">
+        <f>'Sprint Backlog'!H14</f>
+        <v>7.5</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>5</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15">
+        <f>'Sprint Backlog'!B15</f>
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <f>'Sprint Backlog'!A15</f>
+        <v>2.4</v>
+      </c>
+      <c r="C15">
+        <f>'Sprint Backlog'!H15</f>
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16">
+        <f>'Sprint Backlog'!B16</f>
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <f>'Sprint Backlog'!A16</f>
+        <v>0.1</v>
+      </c>
+      <c r="C16">
+        <f>'Sprint Backlog'!H16</f>
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17">
+        <f>'Sprint Backlog'!B17</f>
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <f>'Sprint Backlog'!A17</f>
+        <v>2.5</v>
+      </c>
+      <c r="C17">
+        <f>'Sprint Backlog'!H17</f>
+        <v>0.5</v>
+      </c>
+      <c r="I17">
+        <v>0.5</v>
+      </c>
+      <c r="J17">
+        <v>0.5</v>
+      </c>
+      <c r="K17">
+        <v>0.5</v>
+      </c>
+      <c r="L17">
+        <v>0.5</v>
+      </c>
+      <c r="M17">
+        <v>0.5</v>
+      </c>
+      <c r="N17">
+        <v>0.5</v>
+      </c>
+      <c r="O17">
+        <v>0.5</v>
+      </c>
+      <c r="P17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18">
+        <f>'Sprint Backlog'!B18</f>
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <f>'Sprint Backlog'!A18</f>
+        <v>0.2</v>
+      </c>
+      <c r="C18">
+        <f>'Sprint Backlog'!H18</f>
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19">
+        <f>'Sprint Backlog'!B19</f>
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <f>'Sprint Backlog'!A19</f>
+        <v>2.6</v>
+      </c>
+      <c r="C19">
+        <f>'Sprint Backlog'!H19</f>
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20">
+        <f>'Sprint Backlog'!B20</f>
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <f>'Sprint Backlog'!A20</f>
+        <v>2.7</v>
+      </c>
+      <c r="C20">
+        <f>'Sprint Backlog'!H20</f>
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21">
+        <f>'Sprint Backlog'!B21</f>
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <f>'Sprint Backlog'!A21</f>
+        <v>3.1</v>
+      </c>
+      <c r="C21">
+        <f>'Sprint Backlog'!H21</f>
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22">
+        <f>'Sprint Backlog'!B22</f>
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <f>'Sprint Backlog'!A22</f>
+        <v>3.2</v>
+      </c>
+      <c r="C22">
+        <f>'Sprint Backlog'!H22</f>
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+      <c r="M22">
+        <v>4</v>
+      </c>
+      <c r="N22">
+        <v>4</v>
+      </c>
+      <c r="O22">
+        <v>4</v>
+      </c>
+      <c r="P22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23">
+        <f>'Sprint Backlog'!B23</f>
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <f>'Sprint Backlog'!A23</f>
+        <v>0.3</v>
+      </c>
+      <c r="C23">
+        <f>'Sprint Backlog'!H23</f>
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>2.5</v>
+      </c>
+      <c r="L23">
+        <v>2.5</v>
+      </c>
+      <c r="M23">
+        <v>2.5</v>
+      </c>
+      <c r="N23">
+        <v>2.5</v>
+      </c>
+      <c r="O23">
+        <v>2.5</v>
+      </c>
+      <c r="P23">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24">
+        <f>'Sprint Backlog'!B24</f>
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <f>'Sprint Backlog'!A24</f>
+        <v>2.4</v>
+      </c>
+      <c r="C24">
+        <f>'Sprint Backlog'!H24</f>
+        <v>6</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>4</v>
+      </c>
+      <c r="P24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25">
+        <f>'Sprint Backlog'!B25</f>
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <f>'Sprint Backlog'!A25</f>
+        <v>3.1</v>
+      </c>
+      <c r="C25">
+        <f>'Sprint Backlog'!H25</f>
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26">
+        <f>'Sprint Backlog'!B26</f>
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <f>'Sprint Backlog'!A26</f>
+        <v>0.4</v>
+      </c>
+      <c r="C26">
+        <f>'Sprint Backlog'!H26</f>
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="N26">
+        <v>3</v>
+      </c>
+      <c r="O26">
+        <v>3</v>
+      </c>
+      <c r="P26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27">
+        <f>'Sprint Backlog'!B27</f>
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <f>'Sprint Backlog'!A27</f>
+        <v>0.6</v>
+      </c>
+      <c r="C27">
+        <f>'Sprint Backlog'!H27</f>
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28">
+        <f>'Sprint Backlog'!B28</f>
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <f>'Sprint Backlog'!A28</f>
+        <v>3.3</v>
+      </c>
+      <c r="C28">
+        <f>'Sprint Backlog'!H28</f>
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
+      </c>
+      <c r="O28">
+        <v>3</v>
+      </c>
+      <c r="P28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29">
+        <f>'Sprint Backlog'!B29</f>
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <f>'Sprint Backlog'!A29</f>
+        <v>0.5</v>
+      </c>
+      <c r="C29">
+        <f>'Sprint Backlog'!H29</f>
+        <v>6</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0.5</v>
+      </c>
+      <c r="N29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30">
+        <f>'Sprint Backlog'!B30</f>
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <f>'Sprint Backlog'!A30</f>
+        <v>0.7</v>
+      </c>
+      <c r="C30">
+        <f>'Sprint Backlog'!H30</f>
+        <v>2</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31">
+        <f>'Sprint Backlog'!B31</f>
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <f>'Sprint Backlog'!A31</f>
+        <v>0.8</v>
+      </c>
+      <c r="C31">
+        <f>'Sprint Backlog'!H31</f>
+        <v>2</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32">
+        <f>'Sprint Backlog'!B32</f>
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <f>'Sprint Backlog'!A32</f>
+        <v>0.9</v>
+      </c>
+      <c r="C32">
+        <f>'Sprint Backlog'!H32</f>
+        <v>6</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33">
+        <f>'Sprint Backlog'!B33</f>
+        <v>3</v>
+      </c>
+      <c r="B33" s="8" t="str">
+        <f>'Sprint Backlog'!A33</f>
+        <v>0.10</v>
+      </c>
+      <c r="C33">
+        <f>'Sprint Backlog'!H33</f>
+        <v>3</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34">
+        <f>'Sprint Backlog'!B34</f>
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <f>'Sprint Backlog'!A34</f>
+        <v>3.4</v>
+      </c>
+      <c r="C34">
+        <f>'Sprint Backlog'!H34</f>
+        <v>2</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35">
+        <f>'Sprint Backlog'!B35</f>
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <f>'Sprint Backlog'!A35</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C35">
+        <f>'Sprint Backlog'!H35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36">
+        <f>'Sprint Backlog'!B36</f>
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <f>'Sprint Backlog'!A36</f>
+        <v>4.2</v>
+      </c>
+      <c r="C36">
+        <f>'Sprint Backlog'!H36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" s="12" customFormat="1"/>
+    <row r="38" spans="1:16">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="D38" s="9">
+        <f>D1</f>
+        <v>41398</v>
+      </c>
+      <c r="E38" s="9">
+        <f t="shared" ref="E38:P38" si="0">E1</f>
+        <v>41402</v>
+      </c>
+      <c r="F38" s="9">
+        <f t="shared" si="0"/>
+        <v>41410</v>
+      </c>
+      <c r="G38" s="9">
+        <f t="shared" si="0"/>
+        <v>41411</v>
+      </c>
+      <c r="H38" s="9">
+        <f t="shared" si="0"/>
+        <v>41416</v>
+      </c>
+      <c r="I38" s="9">
+        <f t="shared" si="0"/>
+        <v>41418</v>
+      </c>
+      <c r="J38" s="9">
+        <f t="shared" si="0"/>
+        <v>41423</v>
+      </c>
+      <c r="K38" s="9">
+        <f t="shared" si="0"/>
+        <v>41425</v>
+      </c>
+      <c r="L38" s="9">
+        <f t="shared" si="0"/>
+        <v>41427</v>
+      </c>
+      <c r="M38" s="9">
+        <f t="shared" si="0"/>
+        <v>41430</v>
+      </c>
+      <c r="N38" s="9">
+        <f t="shared" si="0"/>
+        <v>41432</v>
+      </c>
+      <c r="O38" s="9">
+        <f t="shared" si="0"/>
+        <v>41437</v>
+      </c>
+      <c r="P38" s="9">
+        <f t="shared" si="0"/>
+        <v>41439</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="B39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="11">
+        <f>SUM(C2:C36)</f>
+        <v>101.5</v>
+      </c>
+      <c r="D39" s="11">
+        <f>$C$39-(COUNT($D$1:D1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>93.692307692307693</v>
+      </c>
+      <c r="E39" s="11">
+        <f>$C$39-(COUNT($D$1:E1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>85.884615384615387</v>
+      </c>
+      <c r="F39" s="11">
+        <f>$C$39-(COUNT($D$1:F1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>78.07692307692308</v>
+      </c>
+      <c r="G39" s="11">
+        <f>$C$39-(COUNT($D$1:G1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>70.269230769230774</v>
+      </c>
+      <c r="H39" s="11">
+        <f>$C$39-(COUNT($D$1:H1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>62.46153846153846</v>
+      </c>
+      <c r="I39" s="11">
+        <f>$C$39-(COUNT($D$1:I1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>54.653846153846153</v>
+      </c>
+      <c r="J39" s="11">
+        <f>$C$39-(COUNT($D$1:J1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>46.846153846153847</v>
+      </c>
+      <c r="K39" s="11">
+        <f>$C$39-(COUNT($D$1:K1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>39.03846153846154</v>
+      </c>
+      <c r="L39" s="11">
+        <f>$C$39-(COUNT($D$1:L1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>31.230769230769226</v>
+      </c>
+      <c r="M39" s="11">
+        <f>$C$39-(COUNT($D$1:M1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>23.42307692307692</v>
+      </c>
+      <c r="N39" s="11">
+        <f>$C$39-(COUNT($D$1:N1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>15.615384615384613</v>
+      </c>
+      <c r="O39" s="11">
+        <f>$C$39-(COUNT($D$1:O1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>7.8076923076923066</v>
+      </c>
+      <c r="P39" s="11">
+        <f>$C$39-(COUNT($D$1:P1)*$C$39/COUNT($D$1:$P$1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="B40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="11">
+        <f>C39</f>
+        <v>101.5</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11">
+        <f>$C$40-SUM(H2:H36)</f>
+        <v>69.5</v>
+      </c>
+      <c r="I40" s="11">
+        <f>$C$40-SUM(I2:I36)</f>
+        <v>60</v>
+      </c>
+      <c r="J40" s="11">
+        <f>$C$40-SUM(J2:J36)</f>
+        <v>60</v>
+      </c>
+      <c r="K40" s="11">
+        <f>$C$40-SUM(K2:K36)</f>
+        <v>37</v>
+      </c>
+      <c r="L40" s="11">
+        <f>$C$40-SUM(L2:L36)</f>
+        <v>37</v>
+      </c>
+      <c r="M40" s="11">
+        <f>$C$40-SUM(M2:M36)</f>
+        <v>29.5</v>
+      </c>
+      <c r="N40" s="11">
+        <f>$C$40-SUM(N2:N36)</f>
+        <v>26</v>
+      </c>
+      <c r="O40" s="11">
+        <f>$C$40-SUM(O2:O36)</f>
+        <v>28</v>
+      </c>
+      <c r="P40" s="11">
+        <f>$C$40-SUM(P2:P36)</f>
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated scrum document with latest burndown chart
</commit_message>
<xml_diff>
--- a/Project Pink/doc/scrum/scrum.xlsx
+++ b/Project Pink/doc/scrum/scrum.xlsx
@@ -488,8 +488,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -546,7 +550,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -561,6 +565,8 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -575,6 +581,8 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -891,10 +899,10 @@
                   <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.0</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -911,11 +919,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2083303944"/>
-        <c:axId val="-2064237912"/>
+        <c:axId val="1837695816"/>
+        <c:axId val="1837698904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2083303944"/>
+        <c:axId val="1837695816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -925,7 +933,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064237912"/>
+        <c:crossAx val="1837698904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -933,7 +941,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2064237912"/>
+        <c:axId val="1837698904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,7 +956,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2083303944"/>
+        <c:crossAx val="1837695816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1524,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H36"/>
+    <sheetView topLeftCell="A27" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J34" sqref="J2:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2543,10 +2551,10 @@
         <v>6</v>
       </c>
       <c r="J29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="42">
@@ -2578,10 +2586,10 @@
         <v>2</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="28">
@@ -2613,10 +2621,10 @@
         <v>2</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="28">
@@ -2648,10 +2656,10 @@
         <v>6</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="42">
@@ -2683,10 +2691,10 @@
         <v>3</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="28">
@@ -2718,10 +2726,10 @@
         <v>2</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="56">
@@ -2780,8 +2788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="S59" sqref="S59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3860,6 +3868,12 @@
       <c r="N29">
         <v>2</v>
       </c>
+      <c r="O29">
+        <v>2</v>
+      </c>
+      <c r="P29">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30">
@@ -3880,6 +3894,12 @@
       <c r="N30">
         <v>0</v>
       </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31">
@@ -3900,6 +3920,12 @@
       <c r="N31">
         <v>0</v>
       </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32">
@@ -3920,6 +3946,12 @@
       <c r="N32">
         <v>0</v>
       </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>3</v>
+      </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33">
@@ -3940,6 +3972,12 @@
       <c r="N33">
         <v>0</v>
       </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:16">
       <c r="A34">
@@ -3956,6 +3994,12 @@
       </c>
       <c r="N34">
         <v>0</v>
+      </c>
+      <c r="O34">
+        <v>2</v>
+      </c>
+      <c r="P34">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -4117,40 +4161,40 @@
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11">
-        <f>$C$40-SUM(H2:H36)</f>
+        <f t="shared" ref="H40:P40" si="1">$C$40-SUM(H2:H36)</f>
         <v>69.5</v>
       </c>
       <c r="I40" s="11">
-        <f>$C$40-SUM(I2:I36)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="J40" s="11">
-        <f>$C$40-SUM(J2:J36)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="K40" s="11">
-        <f>$C$40-SUM(K2:K36)</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="L40" s="11">
-        <f>$C$40-SUM(L2:L36)</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="M40" s="11">
-        <f>$C$40-SUM(M2:M36)</f>
+        <f t="shared" si="1"/>
         <v>29.5</v>
       </c>
       <c r="N40" s="11">
-        <f>$C$40-SUM(N2:N36)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="O40" s="11">
-        <f>$C$40-SUM(O2:O36)</f>
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
       <c r="P40" s="11">
-        <f>$C$40-SUM(P2:P36)</f>
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>